<commit_message>
fixed all the figures
</commit_message>
<xml_diff>
--- a/crowd_certain/outputs/final_figures/figure_heatmap_F_evals_all_datasets_NL3/figure_heatmap_F_evals_all_datasets_NL3.xlsx
+++ b/crowd_certain/outputs/final_figures/figure_heatmap_F_evals_all_datasets_NL3/figure_heatmap_F_evals_all_datasets_NL3.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.188</v>
+        <v>2.204</v>
       </c>
       <c r="D5" t="n">
         <v>3.092</v>
@@ -599,7 +599,7 @@
         <v>2.391</v>
       </c>
       <c r="F5" t="n">
-        <v>2.25</v>
+        <v>2.322</v>
       </c>
       <c r="G5" t="n">
         <v>1.963</v>
@@ -609,483 +609,67 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n"/>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>brier score loss</t>
+        </is>
+      </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>iris</t>
+          <t>kr-vs-kp</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.263</v>
+        <v>0.781</v>
       </c>
       <c r="D6" t="n">
-        <v>3.342</v>
+        <v>0.445</v>
       </c>
       <c r="E6" t="n">
-        <v>2.485</v>
+        <v>0.428</v>
       </c>
       <c r="F6" t="n">
-        <v>3.225</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>2.153</v>
+        <v>0.446</v>
       </c>
       <c r="H6" t="n">
-        <v>2.403</v>
+        <v>0.414</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>spambase</t>
+          <t>mushroom</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.336</v>
+        <v>0.956</v>
       </c>
       <c r="D7" t="n">
-        <v>3.124</v>
+        <v>0.453</v>
       </c>
       <c r="E7" t="n">
-        <v>2.428</v>
+        <v>0.435</v>
       </c>
       <c r="F7" t="n">
-        <v>2.084</v>
+        <v>0.725</v>
       </c>
       <c r="G7" t="n">
-        <v>2.144</v>
+        <v>0.478</v>
       </c>
       <c r="H7" t="n">
-        <v>3.306</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>tic-tac-toe</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>2.497</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3.104</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2.385</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2.413</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2.065</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3.253</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>sick</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1.352</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3.104</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2.377</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.166</v>
-      </c>
-      <c r="G9" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="H9" t="n">
-        <v>3.164</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>waveform</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2.374</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2.979</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2.286</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2.163</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1.982</v>
-      </c>
-      <c r="H10" t="n">
-        <v>3.169</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>2.514</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2.387</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2.359</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2.731</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3.266</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>vote</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>2.641</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3.367</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2.586</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2.804</v>
-      </c>
-      <c r="G12" t="n">
-        <v>2.627</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2.533</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>ionosphere</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>3.075</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2.963</v>
-      </c>
-      <c r="E13" t="n">
-        <v>2.117</v>
-      </c>
-      <c r="F13" t="n">
-        <v>3.298</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1.839</v>
-      </c>
-      <c r="H13" t="n">
-        <v>2.052</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>brier score loss</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>kr-vs-kp</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0.781</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.445</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.428</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.6840000000000001</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.446</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.414</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>mushroom</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0.955</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.453</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.435</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.725</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.478</v>
-      </c>
-      <c r="H15" t="n">
         <v>0.421</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n"/>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>iris</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0.618</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.455</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.598</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.469</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.433</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>spambase</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.833</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.453</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.436</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.702</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.504</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.422</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>tic-tac-toe</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0.582</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.441</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.613</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.514</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.425</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>sick</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0.9370000000000001</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.451</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.433</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.5629999999999999</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.419</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>waveform</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0.843</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.434</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.654</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.468</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.419</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0.747</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.458</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.439</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.699</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.522</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.425</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>vote</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0.873</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.434</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.726</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.511</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>ionosphere</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.428</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.414</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.485</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.385</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A4:A13"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed issues. worked on parallelization
</commit_message>
<xml_diff>
--- a/crowd_certain/outputs/final_figures/figure_heatmap_F_evals_all_datasets_NL3/figure_heatmap_F_evals_all_datasets_NL3.xlsx
+++ b/crowd_certain/outputs/final_figures/figure_heatmap_F_evals_all_datasets_NL3/figure_heatmap_F_evals_all_datasets_NL3.xlsx
@@ -564,22 +564,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.732</v>
+        <v>2.844</v>
       </c>
       <c r="D4" t="n">
-        <v>3.075</v>
+        <v>3.105</v>
       </c>
       <c r="E4" t="n">
-        <v>2.398</v>
+        <v>2.388</v>
       </c>
       <c r="F4" t="n">
-        <v>2.289</v>
+        <v>2.464</v>
       </c>
       <c r="G4" t="n">
-        <v>2.104</v>
+        <v>2.141</v>
       </c>
       <c r="H4" t="n">
-        <v>3.272</v>
+        <v>3.269</v>
       </c>
     </row>
     <row r="5">
@@ -590,22 +590,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.204</v>
+        <v>2.647</v>
       </c>
       <c r="D5" t="n">
-        <v>3.092</v>
+        <v>3.098</v>
       </c>
       <c r="E5" t="n">
-        <v>2.391</v>
+        <v>2.37</v>
       </c>
       <c r="F5" t="n">
-        <v>2.322</v>
+        <v>2.809</v>
       </c>
       <c r="G5" t="n">
-        <v>1.963</v>
+        <v>2.012</v>
       </c>
       <c r="H5" t="n">
-        <v>3.267</v>
+        <v>3.252</v>
       </c>
     </row>
     <row r="6">
@@ -620,22 +620,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.781</v>
+        <v>0.752</v>
       </c>
       <c r="D6" t="n">
-        <v>0.445</v>
+        <v>0.461</v>
       </c>
       <c r="E6" t="n">
+        <v>0.443</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.648</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.428</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.6840000000000001</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.446</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.414</v>
       </c>
     </row>
     <row r="7">
@@ -646,22 +646,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.956</v>
+        <v>0.966</v>
       </c>
       <c r="D7" t="n">
-        <v>0.453</v>
+        <v>0.458</v>
       </c>
       <c r="E7" t="n">
-        <v>0.435</v>
+        <v>0.438</v>
       </c>
       <c r="F7" t="n">
-        <v>0.725</v>
+        <v>0.728</v>
       </c>
       <c r="G7" t="n">
-        <v>0.478</v>
+        <v>0.485</v>
       </c>
       <c r="H7" t="n">
-        <v>0.421</v>
+        <v>0.426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed all the issues related to enum classes
</commit_message>
<xml_diff>
--- a/crowd_certain/outputs/final_figures/figure_heatmap_F_evals_all_datasets_NL3/figure_heatmap_F_evals_all_datasets_NL3.xlsx
+++ b/crowd_certain/outputs/final_figures/figure_heatmap_F_evals_all_datasets_NL3/figure_heatmap_F_evals_all_datasets_NL3.xlsx
@@ -564,22 +564,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.844</v>
+        <v>2.253</v>
       </c>
       <c r="D4" t="n">
-        <v>3.105</v>
+        <v>1.807</v>
       </c>
       <c r="E4" t="n">
-        <v>2.388</v>
+        <v>1.04</v>
       </c>
       <c r="F4" t="n">
-        <v>2.464</v>
+        <v>1.653</v>
       </c>
       <c r="G4" t="n">
-        <v>2.141</v>
+        <v>1.083</v>
       </c>
       <c r="H4" t="n">
-        <v>3.269</v>
+        <v>1.878</v>
       </c>
     </row>
     <row r="5">
@@ -590,22 +590,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.647</v>
+        <v>1.351</v>
       </c>
       <c r="D5" t="n">
-        <v>3.098</v>
+        <v>1.882</v>
       </c>
       <c r="E5" t="n">
-        <v>2.37</v>
+        <v>1.115</v>
       </c>
       <c r="F5" t="n">
-        <v>2.809</v>
+        <v>1.63</v>
       </c>
       <c r="G5" t="n">
-        <v>2.012</v>
+        <v>1.228</v>
       </c>
       <c r="H5" t="n">
-        <v>3.252</v>
+        <v>1.957</v>
       </c>
     </row>
     <row r="6">
@@ -620,22 +620,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.752</v>
+        <v>0.773</v>
       </c>
       <c r="D6" t="n">
-        <v>0.461</v>
+        <v>0.412</v>
       </c>
       <c r="E6" t="n">
-        <v>0.443</v>
+        <v>0.394</v>
       </c>
       <c r="F6" t="n">
-        <v>0.648</v>
+        <v>0.633</v>
       </c>
       <c r="G6" t="n">
-        <v>0.488</v>
+        <v>0.431</v>
       </c>
       <c r="H6" t="n">
-        <v>0.428</v>
+        <v>0.384</v>
       </c>
     </row>
     <row r="7">
@@ -646,22 +646,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.966</v>
+        <v>0.959</v>
       </c>
       <c r="D7" t="n">
-        <v>0.458</v>
+        <v>0.428</v>
       </c>
       <c r="E7" t="n">
-        <v>0.438</v>
+        <v>0.412</v>
       </c>
       <c r="F7" t="n">
-        <v>0.728</v>
+        <v>0.674</v>
       </c>
       <c r="G7" t="n">
-        <v>0.485</v>
+        <v>0.457</v>
       </c>
       <c r="H7" t="n">
-        <v>0.426</v>
+        <v>0.398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>